<commit_message>
Added Excel_Range Module Object
</commit_message>
<xml_diff>
--- a/Lib/thinBasic_Excel/Excel_Test_SingleWorkBook.tbasic.xlsx
+++ b/Lib/thinBasic_Excel/Excel_Test_SingleWorkBook.tbasic.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="21285" windowHeight="11790"/>
   </bookViews>
   <sheets>
-    <sheet name="thinBasic_Test_36209_413" sheetId="1" r:id="rId1"/>
+    <sheet name="thinBasic_Test_77110_64" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +29,7 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Few random number</t>
+    <t>Few random numbers</t>
   </si>
 </sst>
 </file>
@@ -65,8 +65,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -352,188 +355,191 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1">
-        <v>1351</v>
-      </c>
-      <c r="D1">
+        <v>845</v>
+      </c>
+      <c r="D1" s="1">
         <f t="shared" ref="D1:D20" si="0">SIN(B1)</f>
-        <v>0.11490459339101296</v>
+        <v>8.8308633096071482E-2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2">
-        <v>1620</v>
-      </c>
-      <c r="D2">
-        <f t="shared" si="0"/>
-        <v>-0.87323854703602033</v>
+        <v>761</v>
+      </c>
+      <c r="D2" s="1">
+        <f t="shared" si="0"/>
+        <v>0.67027391814201598</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>1376</v>
-      </c>
-      <c r="D3">
-        <f t="shared" si="0"/>
-        <v>-1.7581366457004116E-2</v>
+        <v>137</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.94251445455825089</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>1992</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>0.22822835586752283</v>
+        <v>1486</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>-2.6671688735270749E-2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>1905</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>0.93016129842018391</v>
+        <v>750</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.74507295029202647</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6">
-        <v>35</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>-0.42818266949615102</v>
+        <v>242</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>-9.7211907518224325E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7">
-        <v>279</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>0.56608278770604425</v>
+        <v>1899</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.99570095897306632</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8">
-        <v>471</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>-0.23663210523844544</v>
+        <v>1220</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.87335603469517575</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9">
-        <v>677</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>-0.99991265872798241</v>
+        <v>822</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.88996811296178902</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10">
-        <v>416</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>0.96612554987636234</v>
+        <v>582</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.72107948298431912</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11">
-        <v>1599</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>7.0601891231209163E-2</v>
+        <v>273</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.31320015487066988</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12">
-        <v>1401</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>-0.14975799312818225</v>
+        <v>119</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.37140410143809022</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13">
-        <v>1039</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
-        <v>0.7624999444675773</v>
+        <v>1481</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.96614888421283684</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14">
-        <v>1516</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
-        <v>0.98356598244736515</v>
+        <v>1347</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>0.67668318375398939</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15">
-        <v>1612</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="0"/>
-        <v>-0.35505108165397298</v>
+        <v>1814</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.96383556423051653</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16">
-        <v>161</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="0"/>
-        <v>-0.70240778557737105</v>
+        <v>457</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.99482985314176431</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17">
-        <v>1579</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="0"/>
-        <v>0.93947842774886259</v>
+        <v>494</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.69610177347205615</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18">
-        <v>655</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="0"/>
-        <v>0.999756505535219</v>
+        <v>453</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5734065686442813</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19">
-        <v>364</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="0"/>
-        <v>-0.41209101962194344</v>
+        <v>1179</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.7850364106161789</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20">
-        <v>62</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="0"/>
-        <v>-0.73918069664922281</v>
+        <v>379</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="0"/>
+        <v>0.9055655749932976</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -542,11 +548,11 @@
       </c>
       <c r="B22">
         <f>SUM(B1:B20)</f>
-        <v>20110</v>
+        <v>16740</v>
       </c>
       <c r="D22">
         <f>SUM(D1:D20)</f>
-        <v>1.6473694131050638</v>
+        <v>-1.6132342564087025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Excel_Range Font interaction
</commit_message>
<xml_diff>
--- a/Lib/thinBasic_Excel/Excel_Test_SingleWorkBook.tbasic.xlsx
+++ b/Lib/thinBasic_Excel/Excel_Test_SingleWorkBook.tbasic.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="21285" windowHeight="11790"/>
   </bookViews>
   <sheets>
-    <sheet name="thinBasic_Test_77110_64" sheetId="1" r:id="rId1"/>
+    <sheet name="thinBasic_Test_75768_863" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -36,7 +36,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -44,13 +44,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -65,11 +80,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -364,198 +380,199 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>845</v>
+        <v>253</v>
       </c>
       <c r="D1" s="1">
         <f t="shared" ref="D1:D20" si="0">SIN(B1)</f>
-        <v>8.8308633096071482E-2</v>
+        <v>0.99482372867106728</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2">
-        <v>761</v>
+        <v>340</v>
       </c>
       <c r="D2" s="1">
         <f t="shared" si="0"/>
-        <v>0.67027391814201598</v>
+        <v>0.65031074016255253</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>137</v>
+        <v>1861</v>
       </c>
       <c r="D3" s="1">
         <f t="shared" si="0"/>
-        <v>-0.94251445455825089</v>
+        <v>0.92351626822226351</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>1486</v>
+        <v>1831</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" si="0"/>
-        <v>-2.6671688735270749E-2</v>
+        <v>0.52142239732122597</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>750</v>
+        <v>247</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" si="0"/>
-        <v>0.74507295029202647</v>
+        <v>0.92680718550268837</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6">
-        <v>242</v>
+        <v>112</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="0"/>
-        <v>-9.7211907518224325E-2</v>
+        <v>-0.88999560436683334</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7">
-        <v>1899</v>
+        <v>214</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="0"/>
-        <v>0.99570095897306632</v>
+        <v>0.36319945137636067</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8">
-        <v>1220</v>
+        <v>1478</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
-        <v>0.87335603469517575</v>
+        <v>0.99288701129932577</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9">
-        <v>822</v>
+        <v>312</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="0"/>
-        <v>-0.88996811296178902</v>
+        <v>-0.83179147578220447</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10">
-        <v>582</v>
+        <v>920</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="0"/>
-        <v>-0.72107948298431912</v>
+        <v>0.46766522966301216</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11">
-        <v>273</v>
+        <v>1095</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="0"/>
-        <v>0.31320015487066988</v>
+        <v>0.98801767062211421</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12">
-        <v>119</v>
+        <v>1990</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="0"/>
-        <v>-0.37140410143809022</v>
+        <v>-0.98027542118069533</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13">
-        <v>1481</v>
+        <v>1249</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="0"/>
-        <v>-0.96614888421283684</v>
+        <v>-0.97656492400741579</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14">
-        <v>1347</v>
+        <v>1034</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="0"/>
-        <v>0.67668318375398939</v>
+        <v>-0.40412036662142653</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15">
-        <v>1814</v>
+        <v>519</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="0"/>
-        <v>-0.96383556423051653</v>
+        <v>-0.59495700704438548</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16">
-        <v>457</v>
+        <v>364</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="0"/>
-        <v>-0.99482985314176431</v>
+        <v>-0.41209101962194344</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17">
-        <v>494</v>
+        <v>455</v>
       </c>
       <c r="D17" s="1">
         <f t="shared" si="0"/>
-        <v>-0.69610177347205615</v>
+        <v>0.50633964683490129</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18">
-        <v>453</v>
+        <v>1223</v>
       </c>
       <c r="D18" s="1">
         <f t="shared" si="0"/>
-        <v>0.5734065686442813</v>
+        <v>-0.79587885301190697</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19">
-        <v>1179</v>
+        <v>1048</v>
       </c>
       <c r="D19" s="1">
         <f t="shared" si="0"/>
-        <v>-0.7850364106161789</v>
+        <v>-0.9613726040856847</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20">
-        <v>379</v>
+        <v>482</v>
       </c>
       <c r="D20" s="1">
         <f t="shared" si="0"/>
-        <v>0.9055655749932976</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-0.97263707111538011</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>0</v>
       </c>
       <c r="B22">
         <f>SUM(B1:B20)</f>
-        <v>16740</v>
-      </c>
-      <c r="D22">
+        <v>17027</v>
+      </c>
+      <c r="D22" s="2">
         <f>SUM(D1:D20)</f>
-        <v>-1.6132342564087025</v>
+        <v>-0.48469501716236418</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Improved Range and Application interfaces
</commit_message>
<xml_diff>
--- a/Lib/thinBasic_Excel/Excel_Test_SingleWorkBook.tbasic.xlsx
+++ b/Lib/thinBasic_Excel/Excel_Test_SingleWorkBook.tbasic.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="21285" windowHeight="11790"/>
   </bookViews>
   <sheets>
-    <sheet name="thinBasic_Test_64451_117" sheetId="1" r:id="rId1"/>
+    <sheet name="thinBasic_Test_58602_255" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -385,182 +385,182 @@
         <v>0</v>
       </c>
       <c r="B1" s="3">
-        <v>1173</v>
+        <v>1618</v>
       </c>
       <c r="D1" s="1">
         <f t="shared" ref="D1:D20" si="0">SIN(B1)</f>
-        <v>-0.92685246010993383</v>
+        <v>-7.969878609913976E-2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="3">
-        <v>483</v>
+        <v>1594</v>
       </c>
       <c r="D2" s="1">
         <f t="shared" si="0"/>
-        <v>-0.72101682327763728</v>
+        <v>-0.93650426227593253</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="3">
-        <v>201</v>
+        <v>467</v>
       </c>
       <c r="D3" s="1">
         <f t="shared" si="0"/>
-        <v>-6.189025071872073E-2</v>
+        <v>0.88998185906866645</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
-        <v>1097</v>
+        <v>757</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" si="0"/>
-        <v>-0.55150212035805679</v>
+        <v>0.12351329589860736</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
-        <v>1727</v>
+        <v>1520</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" si="0"/>
-        <v>-0.76815816891192723</v>
+        <v>-0.50626166124981298</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
-        <v>843</v>
+        <v>154</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="0"/>
-        <v>0.86899558984115421</v>
+        <v>-6.1920337256057306E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
-        <v>954</v>
+        <v>1047</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="0"/>
-        <v>-0.86450599845484721</v>
+        <v>-0.75104695816131239</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
-        <v>940</v>
+        <v>1745</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
-        <v>-0.61611169210333949</v>
+        <v>-0.98805486192125302</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
-        <v>1763</v>
+        <v>1873</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="0"/>
-        <v>-0.5367000990648747</v>
+        <v>0.57350535004904812</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
-        <v>1692</v>
+        <v>1831</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="0"/>
-        <v>0.9683268389736619</v>
+        <v>0.52142239732122597</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
-        <v>1445</v>
+        <v>1785</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="0"/>
-        <v>-0.13223223246467236</v>
+        <v>0.5441475710529643</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
-        <v>740</v>
+        <v>809</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="0"/>
-        <v>-0.98802232267682955</v>
+        <v>-0.99920443162105288</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
-        <v>480</v>
+        <v>824</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="0"/>
-        <v>0.61601671376416356</v>
+        <v>0.78501773735121527</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
-        <v>1069</v>
+        <v>1300</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="0"/>
-        <v>0.75686160320607432</v>
+        <v>-0.58051300815631324</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
-        <v>1505</v>
+        <v>1205</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="0"/>
-        <v>-0.17619431225785259</v>
+        <v>-0.98022176654524318</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
-        <v>1610</v>
+        <v>384</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="0"/>
-        <v>0.99780726653659702</v>
+        <v>0.66365643362195958</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
-        <v>784</v>
+        <v>1421</v>
       </c>
       <c r="D17" s="1">
         <f t="shared" si="0"/>
-        <v>-0.98513590606142243</v>
+        <v>0.84153612694522806</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
-        <v>1651</v>
+        <v>1471</v>
       </c>
       <c r="D18" s="1">
         <f t="shared" si="0"/>
-        <v>-0.99567299218622052</v>
+        <v>0.67031865800439361</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
-        <v>635</v>
+        <v>1511</v>
       </c>
       <c r="D19" s="1">
         <f t="shared" si="0"/>
-        <v>0.38783720589663306</v>
+        <v>0.10586761272451208</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
-        <v>777</v>
+        <v>1006</v>
       </c>
       <c r="D20" s="1">
         <f t="shared" si="0"/>
-        <v>-0.85555119309212424</v>
+        <v>0.63680773567951732</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
@@ -569,11 +569,11 @@
       </c>
       <c r="B22" s="3">
         <f>SUM(B1:B20)</f>
-        <v>21569</v>
+        <v>24322</v>
       </c>
       <c r="D22" s="2">
         <f>SUM(D1:D20)</f>
-        <v>-4.5837013535201745</v>
+        <v>0.47234870443122101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>